<commit_message>
Solved Product except self in array
</commit_message>
<xml_diff>
--- a/Neetcode_75/Leetcode_75.xlsx
+++ b/Neetcode_75/Leetcode_75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\jigya\Desktop\Github_Projects\DataStructures_and_Algorithms\Neetcode_75\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE0E31F0-06B8-4249-ADD5-584E365F1F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CEB2862-4F77-4889-B90D-88C200297709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="244">
   <si>
     <t>Video Solution</t>
   </si>
@@ -746,6 +746,12 @@
   </si>
   <si>
     <t>initialize a maxprofit and minprice, change the minprice if the current price is lower than the min price and calculate max profit based on price[i] minus minprice</t>
+  </si>
+  <si>
+    <t>Create a hashtable and then iterate through the array, every time you iterate through the array, check if the entry exists in hash table, if exists return true, else add the number to the hash table</t>
+  </si>
+  <si>
+    <t>We use the concept of prefix and suffix product, in the first pass through the output array, we store the prefix product and then we multiply the answer with the post fix product in the output array</t>
   </si>
 </sst>
 </file>
@@ -1252,7 +1258,7 @@
   <dimension ref="A1:E1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1342,7 +1348,9 @@
       <c r="D6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="23"/>
+      <c r="E6" s="23" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
@@ -1357,7 +1365,9 @@
       <c r="D7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="23"/>
+      <c r="E7" s="23" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">

</xml_diff>